<commit_message>
Defined Inclusive logic and plots
</commit_message>
<xml_diff>
--- a/Plots/Workbook1.xlsx
+++ b/Plots/Workbook1.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="53">
   <si>
     <t>8 KiB</t>
   </si>
@@ -157,10 +158,7 @@
     <t>Non-Inclu</t>
   </si>
   <si>
-    <t>L1 Cache Size</t>
-  </si>
-  <si>
-    <t>L1 AMAT</t>
+    <t>L1 Cache Miss Rates</t>
   </si>
   <si>
     <t>Log2 Cache Size(bytes)</t>
@@ -185,6 +183,12 @@
   </si>
   <si>
     <t xml:space="preserve"> FA</t>
+  </si>
+  <si>
+    <t>L1 AMAT (ns)</t>
+  </si>
+  <si>
+    <t>L1 Associativity</t>
   </si>
 </sst>
 </file>
@@ -274,7 +278,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -358,8 +362,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -371,8 +384,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -421,18 +442,32 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4900,6 +4935,658 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1"/>
+              <a:t>Plot</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
+              <a:t> #2a - AMAT vs L1 Cache Size</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GCC.t</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$A$12:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$12:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0134965</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.789956</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7613645</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7651405</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MCF.t</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$A$12:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$C$12:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.33633</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.163061000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.940155</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.956807</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$D$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LBM.t</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$A$12:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$D$12:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.765495</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.316552</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.395159</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.41242</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1542215264"/>
+        <c:axId val="1659499056"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1542215264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="1"/>
+                  <a:t>L1 Associativity</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.451609798775153"/>
+              <c:y val="0.775346675415573"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1659499056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1659499056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="9.0"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="1"/>
+                  <a:t>AMAT (ns)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0194444444444444"/>
+              <c:y val="0.265396981627297"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1542215264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5180,6 +5867,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -8199,6 +8926,509 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8908,6 +10138,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>755650</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>374650</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10689,6 +11954,258 @@
 </a:themeOverride>
 </file>
 
+<file path=xl/theme/themeOverride7.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4472C4"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="Yu Gothic Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="DengXian Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="Yu Gothic"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="DengXian"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AA255"/>
@@ -12986,1270 +14503,1349 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q56"/>
+  <dimension ref="A1:M56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="11" max="11" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="13"/>
-      <c r="K1" t="s">
+      <c r="H1" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Q1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="13"/>
+      <c r="G2">
+        <f>LOG(H:H,2)</f>
+        <v>10</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1024</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>64</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.114797</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <f>LOG(H:H,2)</f>
+        <v>10</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1024</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>64</v>
+      </c>
+      <c r="K3" s="1">
+        <v>2</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.14032899999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
+      <c r="B4" s="10">
+        <v>2.6901499999999998E-2</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.27941300000000002</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.121798</v>
+      </c>
+      <c r="G4">
+        <f>LOG(H:H,2)</f>
+        <v>10</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1024</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>64</v>
+      </c>
+      <c r="K4" s="1">
+        <v>4</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.14682000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>2</v>
+      </c>
+      <c r="B5" s="10">
+        <v>1.8190000000000001E-2</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0.27243499999999998</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.105314</v>
+      </c>
+      <c r="G5">
+        <f>LOG(H:H,2)</f>
+        <v>10</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1024</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>64</v>
+      </c>
+      <c r="K5" s="1">
+        <v>8</v>
+      </c>
+      <c r="L5" s="17">
+        <v>0.178591</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10">
+        <v>1.6900499999999999E-2</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.26444499999999999</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.107721</v>
+      </c>
+      <c r="G6">
+        <f>LOG(H:H,2)</f>
+        <v>10</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1024</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>64</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="L6" s="1">
+        <v>0.15548399999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>8</v>
+      </c>
+      <c r="B7" s="10">
+        <v>1.6435499999999999E-2</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.26442399999999999</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.107721</v>
+      </c>
+      <c r="G7">
+        <f>LOG(H:H,2)</f>
+        <v>11</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2048</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1">
+        <v>64</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.12909000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <f>LOG(H:H,2)</f>
+        <v>11</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2048</v>
+      </c>
+      <c r="I8" s="1">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1">
+        <v>64</v>
+      </c>
+      <c r="K8" s="1">
+        <v>2</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.161691</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f>LOG(H:H,2)</f>
+        <v>11</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2048</v>
+      </c>
+      <c r="I9" s="1">
+        <v>2</v>
+      </c>
+      <c r="J9" s="1">
+        <v>64</v>
+      </c>
+      <c r="K9" s="1">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="L9" s="1">
+        <v>0.15449599999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="13"/>
+      <c r="G10">
+        <f>LOG(H:H,2)</f>
+        <v>11</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2048</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1">
+        <v>64</v>
+      </c>
+      <c r="K10" s="1">
+        <v>8</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0.18068599999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K2">
-        <f t="shared" ref="K2:K56" si="0">LOG(L:L,2)</f>
-        <v>10</v>
-      </c>
-      <c r="L2" s="1">
+      <c r="G11">
+        <f>LOG(H:H,2)</f>
+        <v>11</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2048</v>
+      </c>
+      <c r="I11" s="1">
+        <v>2</v>
+      </c>
+      <c r="J11" s="1">
+        <v>64</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0.17651500000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="19">
+        <v>1</v>
+      </c>
+      <c r="B12" s="10">
+        <v>1.0134965</v>
+      </c>
+      <c r="C12" s="10">
+        <v>8.3363300000000002</v>
+      </c>
+      <c r="D12" s="10">
+        <v>3.765495</v>
+      </c>
+      <c r="G12">
+        <f>LOG(H:H,2)</f>
+        <v>12</v>
+      </c>
+      <c r="H12" s="1">
+        <v>4096</v>
+      </c>
+      <c r="I12" s="1">
+        <v>4</v>
+      </c>
+      <c r="J12" s="1">
+        <v>64</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0.147005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="19">
+        <v>2</v>
+      </c>
+      <c r="B13" s="10">
+        <v>0.78995599999999999</v>
+      </c>
+      <c r="C13" s="10">
+        <v>8.1630610000000008</v>
+      </c>
+      <c r="D13" s="10">
+        <v>3.3165520000000002</v>
+      </c>
+      <c r="G13">
+        <f>LOG(H:H,2)</f>
+        <v>12</v>
+      </c>
+      <c r="H13" s="1">
+        <v>4096</v>
+      </c>
+      <c r="I13" s="1">
+        <v>4</v>
+      </c>
+      <c r="J13" s="1">
+        <v>64</v>
+      </c>
+      <c r="K13" s="1">
+        <v>2</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.18113099999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="19">
+        <v>4</v>
+      </c>
+      <c r="B14" s="10">
+        <v>0.7613645</v>
+      </c>
+      <c r="C14" s="10">
+        <v>7.9401549999999999</v>
+      </c>
+      <c r="D14" s="10">
+        <v>3.395159</v>
+      </c>
+      <c r="G14">
+        <f>LOG(H:H,2)</f>
+        <v>12</v>
+      </c>
+      <c r="H14" s="1">
+        <v>4096</v>
+      </c>
+      <c r="I14" s="1">
+        <v>4</v>
+      </c>
+      <c r="J14" s="1">
+        <v>64</v>
+      </c>
+      <c r="K14" s="1">
+        <v>4</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0.18568499999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="19">
+        <v>8</v>
+      </c>
+      <c r="B15" s="10">
+        <v>0.7651405</v>
+      </c>
+      <c r="C15" s="10">
+        <v>7.9568070000000004</v>
+      </c>
+      <c r="D15" s="10">
+        <v>3.41242</v>
+      </c>
+      <c r="G15">
+        <f>LOG(H:H,2)</f>
+        <v>12</v>
+      </c>
+      <c r="H15" s="1">
+        <v>4096</v>
+      </c>
+      <c r="I15" s="1">
+        <v>4</v>
+      </c>
+      <c r="J15" s="1">
+        <v>64</v>
+      </c>
+      <c r="K15" s="1">
+        <v>8</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0.18906499999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <f>LOG(H:H,2)</f>
+        <v>12</v>
+      </c>
+      <c r="H16" s="1">
+        <v>4096</v>
+      </c>
+      <c r="I16" s="1">
+        <v>4</v>
+      </c>
+      <c r="J16" s="1">
+        <v>64</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0.182948</v>
+      </c>
+    </row>
+    <row r="17" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <f>LOG(H:H,2)</f>
+        <v>13</v>
+      </c>
+      <c r="H17" s="1">
+        <v>8192</v>
+      </c>
+      <c r="I17" s="1">
+        <v>8</v>
+      </c>
+      <c r="J17" s="1">
+        <v>64</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0.16383</v>
+      </c>
+    </row>
+    <row r="18" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <f>LOG(H:H,2)</f>
+        <v>13</v>
+      </c>
+      <c r="H18" s="1">
+        <v>8192</v>
+      </c>
+      <c r="I18" s="1">
+        <v>8</v>
+      </c>
+      <c r="J18" s="1">
+        <v>64</v>
+      </c>
+      <c r="K18" s="1">
+        <v>2</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0.19419499999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <f>LOG(H:H,2)</f>
+        <v>13</v>
+      </c>
+      <c r="H19" s="1">
+        <v>8192</v>
+      </c>
+      <c r="I19" s="1">
+        <v>8</v>
+      </c>
+      <c r="J19" s="1">
+        <v>64</v>
+      </c>
+      <c r="K19" s="1">
+        <v>4</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0.211173</v>
+      </c>
+    </row>
+    <row r="20" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <f>LOG(H:H,2)</f>
+        <v>13</v>
+      </c>
+      <c r="H20" s="1">
+        <v>8192</v>
+      </c>
+      <c r="I20" s="1">
+        <v>8</v>
+      </c>
+      <c r="J20" s="1">
+        <v>64</v>
+      </c>
+      <c r="K20" s="1">
+        <v>8</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0.21291099999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <f>LOG(H:H,2)</f>
+        <v>13</v>
+      </c>
+      <c r="H21" s="1">
+        <v>8192</v>
+      </c>
+      <c r="I21" s="1">
+        <v>8</v>
+      </c>
+      <c r="J21" s="1">
+        <v>64</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0.19858099999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <f>LOG(H:H,2)</f>
+        <v>14</v>
+      </c>
+      <c r="H22" s="1">
+        <v>16384</v>
+      </c>
+      <c r="I22" s="1">
+        <v>16</v>
+      </c>
+      <c r="J22" s="1">
+        <v>64</v>
+      </c>
+      <c r="K22" s="1">
+        <v>1</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0.19841699999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <f>LOG(H:H,2)</f>
+        <v>14</v>
+      </c>
+      <c r="H23" s="1">
+        <v>16384</v>
+      </c>
+      <c r="I23" s="1">
+        <v>16</v>
+      </c>
+      <c r="J23" s="1">
+        <v>64</v>
+      </c>
+      <c r="K23" s="1">
+        <v>2</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0.22391699999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <f>LOG(H:H,2)</f>
+        <v>14</v>
+      </c>
+      <c r="H24" s="1">
+        <v>16384</v>
+      </c>
+      <c r="I24" s="1">
+        <v>16</v>
+      </c>
+      <c r="J24" s="1">
+        <v>64</v>
+      </c>
+      <c r="K24" s="1">
+        <v>4</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0.23393599999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <f>LOG(H:H,2)</f>
+        <v>14</v>
+      </c>
+      <c r="H25" s="1">
+        <v>16384</v>
+      </c>
+      <c r="I25" s="1">
+        <v>16</v>
+      </c>
+      <c r="J25" s="1">
+        <v>64</v>
+      </c>
+      <c r="K25" s="1">
+        <v>8</v>
+      </c>
+      <c r="L25" s="1">
+        <v>0.25435399999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <f>LOG(H:H,2)</f>
+        <v>14</v>
+      </c>
+      <c r="H26" s="1">
+        <v>16384</v>
+      </c>
+      <c r="I26" s="1">
+        <v>16</v>
+      </c>
+      <c r="J26" s="1">
+        <v>64</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L26" s="1">
+        <v>0.20560799999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <f>LOG(H:H,2)</f>
+        <v>15</v>
+      </c>
+      <c r="H27" s="1">
+        <v>32768</v>
+      </c>
+      <c r="I27" s="1">
+        <v>32</v>
+      </c>
+      <c r="J27" s="1">
+        <v>64</v>
+      </c>
+      <c r="K27" s="1">
+        <v>1</v>
+      </c>
+      <c r="L27" s="1">
+        <v>0.23335299999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <f>LOG(H:H,2)</f>
+        <v>15</v>
+      </c>
+      <c r="H28" s="1">
+        <v>32768</v>
+      </c>
+      <c r="I28" s="1">
+        <v>32</v>
+      </c>
+      <c r="J28" s="1">
+        <v>64</v>
+      </c>
+      <c r="K28" s="1">
+        <v>2</v>
+      </c>
+      <c r="L28" s="1">
+        <v>0.26244600000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <f>LOG(H:H,2)</f>
+        <v>15</v>
+      </c>
+      <c r="H29" s="1">
+        <v>32768</v>
+      </c>
+      <c r="I29" s="1">
+        <v>32</v>
+      </c>
+      <c r="J29" s="1">
+        <v>64</v>
+      </c>
+      <c r="K29" s="1">
+        <v>4</v>
+      </c>
+      <c r="L29" s="1">
+        <v>0.27125000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <f>LOG(H:H,2)</f>
+        <v>15</v>
+      </c>
+      <c r="H30" s="1">
+        <v>32768</v>
+      </c>
+      <c r="I30" s="1">
+        <v>32</v>
+      </c>
+      <c r="J30" s="1">
+        <v>64</v>
+      </c>
+      <c r="K30" s="1">
+        <v>8</v>
+      </c>
+      <c r="L30" s="1">
+        <v>0.28851099999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <f>LOG(H:H,2)</f>
+        <v>15</v>
+      </c>
+      <c r="H31" s="1">
+        <v>32768</v>
+      </c>
+      <c r="I31" s="1">
+        <v>32</v>
+      </c>
+      <c r="J31" s="1">
+        <v>64</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L31" s="1">
+        <v>0.22474000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <f>LOG(H:H,2)</f>
+        <v>16</v>
+      </c>
+      <c r="H32" s="1">
+        <v>65536</v>
+      </c>
+      <c r="I32" s="1">
+        <v>64</v>
+      </c>
+      <c r="J32" s="1">
+        <v>64</v>
+      </c>
+      <c r="K32" s="1">
+        <v>1</v>
+      </c>
+      <c r="L32" s="1">
+        <v>0.29462699999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <f>LOG(H:H,2)</f>
+        <v>16</v>
+      </c>
+      <c r="H33" s="1">
+        <v>65536</v>
+      </c>
+      <c r="I33" s="1">
+        <v>64</v>
+      </c>
+      <c r="J33" s="1">
+        <v>64</v>
+      </c>
+      <c r="K33" s="1">
+        <v>2</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0.30072699999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <f>LOG(H:H,2)</f>
+        <v>16</v>
+      </c>
+      <c r="H34" s="1">
+        <v>65536</v>
+      </c>
+      <c r="I34" s="1">
+        <v>64</v>
+      </c>
+      <c r="J34" s="1">
+        <v>64</v>
+      </c>
+      <c r="K34" s="1">
+        <v>4</v>
+      </c>
+      <c r="L34" s="1">
+        <v>0.31948099999999996</v>
+      </c>
+    </row>
+    <row r="35" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <f>LOG(H:H,2)</f>
+        <v>16</v>
+      </c>
+      <c r="H35" s="1">
+        <v>65536</v>
+      </c>
+      <c r="I35" s="1">
+        <v>64</v>
+      </c>
+      <c r="J35" s="1">
+        <v>64</v>
+      </c>
+      <c r="K35" s="1">
+        <v>8</v>
+      </c>
+      <c r="L35" s="1">
+        <v>0.34121299999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <f>LOG(H:H,2)</f>
+        <v>16</v>
+      </c>
+      <c r="H36" s="1">
+        <v>65536</v>
+      </c>
+      <c r="I36" s="1">
+        <v>64</v>
+      </c>
+      <c r="J36" s="1">
+        <v>64</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L36" s="1">
+        <v>0.276281</v>
+      </c>
+    </row>
+    <row r="37" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <f>LOG(H:H,2)</f>
+        <v>17</v>
+      </c>
+      <c r="H37" s="1">
+        <v>131072</v>
+      </c>
+      <c r="I37" s="1">
+        <v>128</v>
+      </c>
+      <c r="J37" s="1">
+        <v>64</v>
+      </c>
+      <c r="K37" s="1">
+        <v>1</v>
+      </c>
+      <c r="L37" s="1">
+        <v>0.36680000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <f>LOG(H:H,2)</f>
+        <v>17</v>
+      </c>
+      <c r="H38" s="1">
+        <v>131072</v>
+      </c>
+      <c r="I38" s="1">
+        <v>128</v>
+      </c>
+      <c r="J38" s="1">
+        <v>64</v>
+      </c>
+      <c r="K38" s="1">
+        <v>2</v>
+      </c>
+      <c r="L38" s="1">
+        <v>0.37460299999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <f>LOG(H:H,2)</f>
+        <v>17</v>
+      </c>
+      <c r="H39" s="1">
+        <v>131072</v>
+      </c>
+      <c r="I39" s="1">
+        <v>128</v>
+      </c>
+      <c r="J39" s="1">
+        <v>64</v>
+      </c>
+      <c r="K39" s="1">
+        <v>4</v>
+      </c>
+      <c r="L39" s="1">
+        <v>0.38028000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <f>LOG(H:H,2)</f>
+        <v>17</v>
+      </c>
+      <c r="H40" s="1">
+        <v>131072</v>
+      </c>
+      <c r="I40" s="1">
+        <v>128</v>
+      </c>
+      <c r="J40" s="1">
+        <v>64</v>
+      </c>
+      <c r="K40" s="1">
+        <v>8</v>
+      </c>
+      <c r="L40" s="1">
+        <v>0.40123599999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <f>LOG(H:H,2)</f>
+        <v>17</v>
+      </c>
+      <c r="H41" s="1">
+        <v>131072</v>
+      </c>
+      <c r="I41" s="1">
+        <v>128</v>
+      </c>
+      <c r="J41" s="1">
+        <v>64</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L41" s="1">
+        <v>0.32248599999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G42">
+        <f>LOG(H:H,2)</f>
+        <v>18</v>
+      </c>
+      <c r="H42" s="1">
+        <v>262144</v>
+      </c>
+      <c r="I42" s="1">
+        <v>256</v>
+      </c>
+      <c r="J42" s="1">
+        <v>64</v>
+      </c>
+      <c r="K42" s="1">
+        <v>1</v>
+      </c>
+      <c r="L42" s="1">
+        <v>0.44381199999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <f>LOG(H:H,2)</f>
+        <v>18</v>
+      </c>
+      <c r="H43" s="1">
+        <v>262144</v>
+      </c>
+      <c r="I43" s="1">
+        <v>256</v>
+      </c>
+      <c r="J43" s="1">
+        <v>64</v>
+      </c>
+      <c r="K43" s="1">
+        <v>2</v>
+      </c>
+      <c r="L43" s="1">
+        <v>0.44592899999999996</v>
+      </c>
+    </row>
+    <row r="44" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G44">
+        <f>LOG(H:H,2)</f>
+        <v>18</v>
+      </c>
+      <c r="H44" s="1">
+        <v>262144</v>
+      </c>
+      <c r="I44" s="1">
+        <v>256</v>
+      </c>
+      <c r="J44" s="1">
+        <v>64</v>
+      </c>
+      <c r="K44" s="1">
+        <v>4</v>
+      </c>
+      <c r="L44" s="1">
+        <v>0.45768499999999995</v>
+      </c>
+    </row>
+    <row r="45" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <f>LOG(H:H,2)</f>
+        <v>18</v>
+      </c>
+      <c r="H45" s="1">
+        <v>262144</v>
+      </c>
+      <c r="I45" s="1">
+        <v>256</v>
+      </c>
+      <c r="J45" s="1">
+        <v>64</v>
+      </c>
+      <c r="K45" s="1">
+        <v>8</v>
+      </c>
+      <c r="L45" s="1">
+        <v>0.45892499999999997</v>
+      </c>
+    </row>
+    <row r="46" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G46">
+        <f>LOG(H:H,2)</f>
+        <v>18</v>
+      </c>
+      <c r="H46" s="1">
+        <v>262144</v>
+      </c>
+      <c r="I46" s="1">
+        <v>256</v>
+      </c>
+      <c r="J46" s="1">
+        <v>64</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L46" s="1">
+        <v>0.396009</v>
+      </c>
+    </row>
+    <row r="47" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G47">
+        <f>LOG(H:H,2)</f>
+        <v>19</v>
+      </c>
+      <c r="H47" s="1">
+        <v>524288</v>
+      </c>
+      <c r="I47" s="1">
+        <v>512</v>
+      </c>
+      <c r="J47" s="1">
+        <v>64</v>
+      </c>
+      <c r="K47" s="1">
+        <v>1</v>
+      </c>
+      <c r="L47" s="1">
+        <v>0.56345099999999992</v>
+      </c>
+    </row>
+    <row r="48" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G48">
+        <f>LOG(H:H,2)</f>
+        <v>19</v>
+      </c>
+      <c r="H48" s="1">
+        <v>524288</v>
+      </c>
+      <c r="I48" s="1">
+        <v>512</v>
+      </c>
+      <c r="J48" s="1">
+        <v>64</v>
+      </c>
+      <c r="K48" s="1">
+        <v>2</v>
+      </c>
+      <c r="L48" s="1">
+        <v>0.56774400000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G49">
+        <f>LOG(H:H,2)</f>
+        <v>19</v>
+      </c>
+      <c r="H49" s="1">
+        <v>524288</v>
+      </c>
+      <c r="I49" s="1">
+        <v>512</v>
+      </c>
+      <c r="J49" s="1">
+        <v>64</v>
+      </c>
+      <c r="K49" s="1">
+        <v>4</v>
+      </c>
+      <c r="L49" s="1">
+        <v>0.56441799999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G50">
+        <f>LOG(H:H,2)</f>
+        <v>19</v>
+      </c>
+      <c r="H50" s="1">
+        <v>524288</v>
+      </c>
+      <c r="I50" s="1">
+        <v>512</v>
+      </c>
+      <c r="J50" s="1">
+        <v>64</v>
+      </c>
+      <c r="K50" s="1">
+        <v>8</v>
+      </c>
+      <c r="L50" s="1">
+        <v>0.57817699999999994</v>
+      </c>
+    </row>
+    <row r="51" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G51">
+        <f>LOG(H:H,2)</f>
+        <v>19</v>
+      </c>
+      <c r="H51" s="1">
+        <v>524288</v>
+      </c>
+      <c r="I51" s="1">
+        <v>512</v>
+      </c>
+      <c r="J51" s="1">
+        <v>64</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L51" s="1">
+        <v>0.47572799999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G52">
+        <f>LOG(H:H,2)</f>
+        <v>20</v>
+      </c>
+      <c r="H52" s="1">
+        <v>1048576</v>
+      </c>
+      <c r="I52" s="1">
         <v>1024</v>
       </c>
-      <c r="M2" s="1">
+      <c r="J52" s="1">
+        <v>64</v>
+      </c>
+      <c r="K52" s="1">
         <v>1</v>
       </c>
-      <c r="N2" s="1">
+      <c r="L52" s="1">
+        <v>0.69938000000000011</v>
+      </c>
+    </row>
+    <row r="53" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G53">
+        <f>LOG(H:H,2)</f>
+        <v>20</v>
+      </c>
+      <c r="H53" s="1">
+        <v>1048576</v>
+      </c>
+      <c r="I53" s="1">
+        <v>1024</v>
+      </c>
+      <c r="J53" s="1">
         <v>64</v>
       </c>
-      <c r="O2" s="1">
-        <v>1</v>
-      </c>
-      <c r="P2" s="1">
-        <v>0.114797</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="10">
-        <v>2.6388000000000002E-2</v>
-      </c>
-      <c r="C3" s="10">
-        <v>0.27941300000000002</v>
-      </c>
-      <c r="D3" s="10">
-        <v>0.107725</v>
-      </c>
-      <c r="K3">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="L3" s="1">
+      <c r="K53" s="1">
+        <v>2</v>
+      </c>
+      <c r="L53" s="1">
+        <v>0.70604599999999995</v>
+      </c>
+    </row>
+    <row r="54" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G54">
+        <f>LOG(H:H,2)</f>
+        <v>20</v>
+      </c>
+      <c r="H54" s="1">
+        <v>1048576</v>
+      </c>
+      <c r="I54" s="1">
         <v>1024</v>
       </c>
-      <c r="M3" s="1">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1">
+      <c r="J54" s="1">
         <v>64</v>
       </c>
-      <c r="O3" s="1">
-        <v>2</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0.14032899999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="10">
-        <v>1.8553E-2</v>
-      </c>
-      <c r="C4" s="10">
-        <v>0.27243499999999998</v>
-      </c>
-      <c r="D4" s="10">
-        <v>0.107721</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="L4" s="1">
+      <c r="K54" s="1">
+        <v>4</v>
+      </c>
+      <c r="L54" s="1">
+        <v>0.69960699999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G55">
+        <f>LOG(H:H,2)</f>
+        <v>20</v>
+      </c>
+      <c r="H55" s="1">
+        <v>1048576</v>
+      </c>
+      <c r="I55" s="1">
         <v>1024</v>
       </c>
-      <c r="M4" s="1">
-        <v>1</v>
-      </c>
-      <c r="N4" s="1">
+      <c r="J55" s="1">
         <v>64</v>
       </c>
-      <c r="O4" s="1">
-        <v>4</v>
-      </c>
-      <c r="P4" s="1">
-        <v>0.14682000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="10">
-        <v>1.6900499999999999E-2</v>
-      </c>
-      <c r="C5" s="10">
-        <v>0.26444499999999999</v>
-      </c>
-      <c r="D5" s="10">
-        <v>0.107721</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="L5" s="1">
+      <c r="K55" s="1">
+        <v>8</v>
+      </c>
+      <c r="L55" s="1">
+        <v>0.70581899999999997</v>
+      </c>
+    </row>
+    <row r="56" spans="7:12" x14ac:dyDescent="0.2">
+      <c r="G56">
+        <f>LOG(H:H,2)</f>
+        <v>20</v>
+      </c>
+      <c r="H56" s="1">
+        <v>1048576</v>
+      </c>
+      <c r="I56" s="1">
         <v>1024</v>
       </c>
-      <c r="M5" s="1">
-        <v>1</v>
-      </c>
-      <c r="N5" s="1">
+      <c r="J56" s="1">
         <v>64</v>
       </c>
-      <c r="O5" s="1">
-        <v>8</v>
-      </c>
-      <c r="P5" s="17">
-        <v>0.178591</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="10">
-        <v>1.6156E-2</v>
-      </c>
-      <c r="C6" s="10">
-        <v>0.247528</v>
-      </c>
-      <c r="D6" s="10">
-        <v>0.101456</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="L6" s="1">
-        <v>1024</v>
-      </c>
-      <c r="M6" s="1">
-        <v>1</v>
-      </c>
-      <c r="N6" s="1">
-        <v>64</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P6" s="1">
-        <v>0.15548399999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="K7">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="L7" s="1">
-        <v>2048</v>
-      </c>
-      <c r="M7" s="1">
-        <v>2</v>
-      </c>
-      <c r="N7" s="1">
-        <v>64</v>
-      </c>
-      <c r="O7" s="1">
-        <v>1</v>
-      </c>
-      <c r="P7" s="1">
-        <v>0.12909000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="K8">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="L8" s="1">
-        <v>2048</v>
-      </c>
-      <c r="M8" s="1">
-        <v>2</v>
-      </c>
-      <c r="N8" s="1">
-        <v>64</v>
-      </c>
-      <c r="O8" s="1">
-        <v>2</v>
-      </c>
-      <c r="P8" s="1">
-        <v>0.161691</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="K9">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="L9" s="1">
-        <v>2048</v>
-      </c>
-      <c r="M9" s="1">
-        <v>2</v>
-      </c>
-      <c r="N9" s="1">
-        <v>64</v>
-      </c>
-      <c r="O9" s="1">
-        <v>4</v>
-      </c>
-      <c r="P9" s="1">
-        <v>0.15449599999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="K10">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="L10" s="1">
-        <v>2048</v>
-      </c>
-      <c r="M10" s="1">
-        <v>2</v>
-      </c>
-      <c r="N10" s="1">
-        <v>64</v>
-      </c>
-      <c r="O10" s="1">
-        <v>8</v>
-      </c>
-      <c r="P10" s="1">
-        <v>0.18068599999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="K11">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="L11" s="1">
-        <v>2048</v>
-      </c>
-      <c r="M11" s="1">
-        <v>2</v>
-      </c>
-      <c r="N11" s="1">
-        <v>64</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P11" s="1">
-        <v>0.17651500000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="K12">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="L12" s="1">
-        <v>4096</v>
-      </c>
-      <c r="M12" s="1">
-        <v>4</v>
-      </c>
-      <c r="N12" s="1">
-        <v>64</v>
-      </c>
-      <c r="O12" s="1">
-        <v>1</v>
-      </c>
-      <c r="P12" s="1">
-        <v>0.147005</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="K13">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="L13" s="1">
-        <v>4096</v>
-      </c>
-      <c r="M13" s="1">
-        <v>4</v>
-      </c>
-      <c r="N13" s="1">
-        <v>64</v>
-      </c>
-      <c r="O13" s="1">
-        <v>2</v>
-      </c>
-      <c r="P13" s="1">
-        <v>0.18113099999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="K14">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="L14" s="1">
-        <v>4096</v>
-      </c>
-      <c r="M14" s="1">
-        <v>4</v>
-      </c>
-      <c r="N14" s="1">
-        <v>64</v>
-      </c>
-      <c r="O14" s="1">
-        <v>4</v>
-      </c>
-      <c r="P14" s="1">
-        <v>0.18568499999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="K15">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="L15" s="1">
-        <v>4096</v>
-      </c>
-      <c r="M15" s="1">
-        <v>4</v>
-      </c>
-      <c r="N15" s="1">
-        <v>64</v>
-      </c>
-      <c r="O15" s="1">
-        <v>8</v>
-      </c>
-      <c r="P15" s="1">
-        <v>0.18906499999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="K16">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="L16" s="1">
-        <v>4096</v>
-      </c>
-      <c r="M16" s="1">
-        <v>4</v>
-      </c>
-      <c r="N16" s="1">
-        <v>64</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P16" s="1">
-        <v>0.182948</v>
-      </c>
-    </row>
-    <row r="17" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K17">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="L17" s="1">
-        <v>8192</v>
-      </c>
-      <c r="M17" s="1">
-        <v>8</v>
-      </c>
-      <c r="N17" s="1">
-        <v>64</v>
-      </c>
-      <c r="O17" s="1">
-        <v>1</v>
-      </c>
-      <c r="P17" s="1">
-        <v>0.16383</v>
-      </c>
-    </row>
-    <row r="18" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K18">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="L18" s="1">
-        <v>8192</v>
-      </c>
-      <c r="M18" s="1">
-        <v>8</v>
-      </c>
-      <c r="N18" s="1">
-        <v>64</v>
-      </c>
-      <c r="O18" s="1">
-        <v>2</v>
-      </c>
-      <c r="P18" s="1">
-        <v>0.19419499999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K19">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="L19" s="1">
-        <v>8192</v>
-      </c>
-      <c r="M19" s="1">
-        <v>8</v>
-      </c>
-      <c r="N19" s="1">
-        <v>64</v>
-      </c>
-      <c r="O19" s="1">
-        <v>4</v>
-      </c>
-      <c r="P19" s="1">
-        <v>0.211173</v>
-      </c>
-    </row>
-    <row r="20" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K20">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="L20" s="1">
-        <v>8192</v>
-      </c>
-      <c r="M20" s="1">
-        <v>8</v>
-      </c>
-      <c r="N20" s="1">
-        <v>64</v>
-      </c>
-      <c r="O20" s="1">
-        <v>8</v>
-      </c>
-      <c r="P20" s="1">
-        <v>0.21291099999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K21">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="L21" s="1">
-        <v>8192</v>
-      </c>
-      <c r="M21" s="1">
-        <v>8</v>
-      </c>
-      <c r="N21" s="1">
-        <v>64</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P21" s="1">
-        <v>0.19858099999999998</v>
-      </c>
-    </row>
-    <row r="22" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K22">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="L22" s="1">
-        <v>16384</v>
-      </c>
-      <c r="M22" s="1">
-        <v>16</v>
-      </c>
-      <c r="N22" s="1">
-        <v>64</v>
-      </c>
-      <c r="O22" s="1">
-        <v>1</v>
-      </c>
-      <c r="P22" s="1">
-        <v>0.19841699999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K23">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="L23" s="1">
-        <v>16384</v>
-      </c>
-      <c r="M23" s="1">
-        <v>16</v>
-      </c>
-      <c r="N23" s="1">
-        <v>64</v>
-      </c>
-      <c r="O23" s="1">
-        <v>2</v>
-      </c>
-      <c r="P23" s="1">
-        <v>0.22391699999999998</v>
-      </c>
-    </row>
-    <row r="24" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K24">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="L24" s="1">
-        <v>16384</v>
-      </c>
-      <c r="M24" s="1">
-        <v>16</v>
-      </c>
-      <c r="N24" s="1">
-        <v>64</v>
-      </c>
-      <c r="O24" s="1">
-        <v>4</v>
-      </c>
-      <c r="P24" s="1">
-        <v>0.23393599999999998</v>
-      </c>
-    </row>
-    <row r="25" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K25">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="L25" s="1">
-        <v>16384</v>
-      </c>
-      <c r="M25" s="1">
-        <v>16</v>
-      </c>
-      <c r="N25" s="1">
-        <v>64</v>
-      </c>
-      <c r="O25" s="1">
-        <v>8</v>
-      </c>
-      <c r="P25" s="1">
-        <v>0.25435399999999997</v>
-      </c>
-    </row>
-    <row r="26" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K26">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="L26" s="1">
-        <v>16384</v>
-      </c>
-      <c r="M26" s="1">
-        <v>16</v>
-      </c>
-      <c r="N26" s="1">
-        <v>64</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P26" s="1">
-        <v>0.20560799999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K27">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="L27" s="1">
-        <v>32768</v>
-      </c>
-      <c r="M27" s="1">
-        <v>32</v>
-      </c>
-      <c r="N27" s="1">
-        <v>64</v>
-      </c>
-      <c r="O27" s="1">
-        <v>1</v>
-      </c>
-      <c r="P27" s="1">
-        <v>0.23335299999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K28">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="L28" s="1">
-        <v>32768</v>
-      </c>
-      <c r="M28" s="1">
-        <v>32</v>
-      </c>
-      <c r="N28" s="1">
-        <v>64</v>
-      </c>
-      <c r="O28" s="1">
-        <v>2</v>
-      </c>
-      <c r="P28" s="1">
-        <v>0.26244600000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K29">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="L29" s="1">
-        <v>32768</v>
-      </c>
-      <c r="M29" s="1">
-        <v>32</v>
-      </c>
-      <c r="N29" s="1">
-        <v>64</v>
-      </c>
-      <c r="O29" s="1">
-        <v>4</v>
-      </c>
-      <c r="P29" s="1">
-        <v>0.27125000000000005</v>
-      </c>
-    </row>
-    <row r="30" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K30">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="L30" s="1">
-        <v>32768</v>
-      </c>
-      <c r="M30" s="1">
-        <v>32</v>
-      </c>
-      <c r="N30" s="1">
-        <v>64</v>
-      </c>
-      <c r="O30" s="1">
-        <v>8</v>
-      </c>
-      <c r="P30" s="1">
-        <v>0.28851099999999996</v>
-      </c>
-    </row>
-    <row r="31" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K31">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="L31" s="1">
-        <v>32768</v>
-      </c>
-      <c r="M31" s="1">
-        <v>32</v>
-      </c>
-      <c r="N31" s="1">
-        <v>64</v>
-      </c>
-      <c r="O31" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P31" s="1">
-        <v>0.22474000000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K32">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="L32" s="1">
-        <v>65536</v>
-      </c>
-      <c r="M32" s="1">
-        <v>64</v>
-      </c>
-      <c r="N32" s="1">
-        <v>64</v>
-      </c>
-      <c r="O32" s="1">
-        <v>1</v>
-      </c>
-      <c r="P32" s="1">
-        <v>0.29462699999999997</v>
-      </c>
-    </row>
-    <row r="33" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K33">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="L33" s="1">
-        <v>65536</v>
-      </c>
-      <c r="M33" s="1">
-        <v>64</v>
-      </c>
-      <c r="N33" s="1">
-        <v>64</v>
-      </c>
-      <c r="O33" s="1">
-        <v>2</v>
-      </c>
-      <c r="P33" s="1">
-        <v>0.30072699999999997</v>
-      </c>
-    </row>
-    <row r="34" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K34">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="L34" s="1">
-        <v>65536</v>
-      </c>
-      <c r="M34" s="1">
-        <v>64</v>
-      </c>
-      <c r="N34" s="1">
-        <v>64</v>
-      </c>
-      <c r="O34" s="1">
-        <v>4</v>
-      </c>
-      <c r="P34" s="1">
-        <v>0.31948099999999996</v>
-      </c>
-    </row>
-    <row r="35" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K35">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="L35" s="1">
-        <v>65536</v>
-      </c>
-      <c r="M35" s="1">
-        <v>64</v>
-      </c>
-      <c r="N35" s="1">
-        <v>64</v>
-      </c>
-      <c r="O35" s="1">
-        <v>8</v>
-      </c>
-      <c r="P35" s="1">
-        <v>0.34121299999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K36">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="L36" s="1">
-        <v>65536</v>
-      </c>
-      <c r="M36" s="1">
-        <v>64</v>
-      </c>
-      <c r="N36" s="1">
-        <v>64</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P36" s="1">
-        <v>0.276281</v>
-      </c>
-    </row>
-    <row r="37" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K37">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="L37" s="1">
-        <v>131072</v>
-      </c>
-      <c r="M37" s="1">
-        <v>128</v>
-      </c>
-      <c r="N37" s="1">
-        <v>64</v>
-      </c>
-      <c r="O37" s="1">
-        <v>1</v>
-      </c>
-      <c r="P37" s="1">
-        <v>0.36680000000000001</v>
-      </c>
-    </row>
-    <row r="38" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K38">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="L38" s="1">
-        <v>131072</v>
-      </c>
-      <c r="M38" s="1">
-        <v>128</v>
-      </c>
-      <c r="N38" s="1">
-        <v>64</v>
-      </c>
-      <c r="O38" s="1">
-        <v>2</v>
-      </c>
-      <c r="P38" s="1">
-        <v>0.37460299999999996</v>
-      </c>
-    </row>
-    <row r="39" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K39">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="L39" s="1">
-        <v>131072</v>
-      </c>
-      <c r="M39" s="1">
-        <v>128</v>
-      </c>
-      <c r="N39" s="1">
-        <v>64</v>
-      </c>
-      <c r="O39" s="1">
-        <v>4</v>
-      </c>
-      <c r="P39" s="1">
-        <v>0.38028000000000001</v>
-      </c>
-    </row>
-    <row r="40" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K40">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="L40" s="1">
-        <v>131072</v>
-      </c>
-      <c r="M40" s="1">
-        <v>128</v>
-      </c>
-      <c r="N40" s="1">
-        <v>64</v>
-      </c>
-      <c r="O40" s="1">
-        <v>8</v>
-      </c>
-      <c r="P40" s="1">
-        <v>0.40123599999999998</v>
-      </c>
-    </row>
-    <row r="41" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K41">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="L41" s="1">
-        <v>131072</v>
-      </c>
-      <c r="M41" s="1">
-        <v>128</v>
-      </c>
-      <c r="N41" s="1">
-        <v>64</v>
-      </c>
-      <c r="O41" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P41" s="1">
-        <v>0.32248599999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K42">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="L42" s="1">
-        <v>262144</v>
-      </c>
-      <c r="M42" s="1">
-        <v>256</v>
-      </c>
-      <c r="N42" s="1">
-        <v>64</v>
-      </c>
-      <c r="O42" s="1">
-        <v>1</v>
-      </c>
-      <c r="P42" s="1">
-        <v>0.44381199999999998</v>
-      </c>
-    </row>
-    <row r="43" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K43">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="L43" s="1">
-        <v>262144</v>
-      </c>
-      <c r="M43" s="1">
-        <v>256</v>
-      </c>
-      <c r="N43" s="1">
-        <v>64</v>
-      </c>
-      <c r="O43" s="1">
-        <v>2</v>
-      </c>
-      <c r="P43" s="1">
-        <v>0.44592899999999996</v>
-      </c>
-    </row>
-    <row r="44" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K44">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="L44" s="1">
-        <v>262144</v>
-      </c>
-      <c r="M44" s="1">
-        <v>256</v>
-      </c>
-      <c r="N44" s="1">
-        <v>64</v>
-      </c>
-      <c r="O44" s="1">
-        <v>4</v>
-      </c>
-      <c r="P44" s="1">
-        <v>0.45768499999999995</v>
-      </c>
-    </row>
-    <row r="45" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K45">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="L45" s="1">
-        <v>262144</v>
-      </c>
-      <c r="M45" s="1">
-        <v>256</v>
-      </c>
-      <c r="N45" s="1">
-        <v>64</v>
-      </c>
-      <c r="O45" s="1">
-        <v>8</v>
-      </c>
-      <c r="P45" s="1">
-        <v>0.45892499999999997</v>
-      </c>
-    </row>
-    <row r="46" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K46">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="L46" s="1">
-        <v>262144</v>
-      </c>
-      <c r="M46" s="1">
-        <v>256</v>
-      </c>
-      <c r="N46" s="1">
-        <v>64</v>
-      </c>
-      <c r="O46" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P46" s="1">
-        <v>0.396009</v>
-      </c>
-    </row>
-    <row r="47" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K47">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="L47" s="1">
-        <v>524288</v>
-      </c>
-      <c r="M47" s="1">
-        <v>512</v>
-      </c>
-      <c r="N47" s="1">
-        <v>64</v>
-      </c>
-      <c r="O47" s="1">
-        <v>1</v>
-      </c>
-      <c r="P47" s="1">
-        <v>0.56345099999999992</v>
-      </c>
-    </row>
-    <row r="48" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K48">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="L48" s="1">
-        <v>524288</v>
-      </c>
-      <c r="M48" s="1">
-        <v>512</v>
-      </c>
-      <c r="N48" s="1">
-        <v>64</v>
-      </c>
-      <c r="O48" s="1">
-        <v>2</v>
-      </c>
-      <c r="P48" s="1">
-        <v>0.56774400000000003</v>
-      </c>
-    </row>
-    <row r="49" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K49">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="L49" s="1">
-        <v>524288</v>
-      </c>
-      <c r="M49" s="1">
-        <v>512</v>
-      </c>
-      <c r="N49" s="1">
-        <v>64</v>
-      </c>
-      <c r="O49" s="1">
-        <v>4</v>
-      </c>
-      <c r="P49" s="1">
-        <v>0.56441799999999998</v>
-      </c>
-    </row>
-    <row r="50" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K50">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="L50" s="1">
-        <v>524288</v>
-      </c>
-      <c r="M50" s="1">
-        <v>512</v>
-      </c>
-      <c r="N50" s="1">
-        <v>64</v>
-      </c>
-      <c r="O50" s="1">
-        <v>8</v>
-      </c>
-      <c r="P50" s="1">
-        <v>0.57817699999999994</v>
-      </c>
-    </row>
-    <row r="51" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K51">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="L51" s="1">
-        <v>524288</v>
-      </c>
-      <c r="M51" s="1">
-        <v>512</v>
-      </c>
-      <c r="N51" s="1">
-        <v>64</v>
-      </c>
-      <c r="O51" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P51" s="1">
-        <v>0.47572799999999998</v>
-      </c>
-    </row>
-    <row r="52" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K52">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="L52" s="1">
-        <v>1048576</v>
-      </c>
-      <c r="M52" s="1">
-        <v>1024</v>
-      </c>
-      <c r="N52" s="1">
-        <v>64</v>
-      </c>
-      <c r="O52" s="1">
-        <v>1</v>
-      </c>
-      <c r="P52" s="1">
-        <v>0.69938000000000011</v>
-      </c>
-    </row>
-    <row r="53" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K53">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="L53" s="1">
-        <v>1048576</v>
-      </c>
-      <c r="M53" s="1">
-        <v>1024</v>
-      </c>
-      <c r="N53" s="1">
-        <v>64</v>
-      </c>
-      <c r="O53" s="1">
-        <v>2</v>
-      </c>
-      <c r="P53" s="1">
-        <v>0.70604599999999995</v>
-      </c>
-    </row>
-    <row r="54" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K54">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="L54" s="1">
-        <v>1048576</v>
-      </c>
-      <c r="M54" s="1">
-        <v>1024</v>
-      </c>
-      <c r="N54" s="1">
-        <v>64</v>
-      </c>
-      <c r="O54" s="1">
-        <v>4</v>
-      </c>
-      <c r="P54" s="1">
-        <v>0.69960699999999998</v>
-      </c>
-    </row>
-    <row r="55" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K55">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="L55" s="1">
-        <v>1048576</v>
-      </c>
-      <c r="M55" s="1">
-        <v>1024</v>
-      </c>
-      <c r="N55" s="1">
-        <v>64</v>
-      </c>
-      <c r="O55" s="1">
-        <v>8</v>
-      </c>
-      <c r="P55" s="1">
-        <v>0.70581899999999997</v>
-      </c>
-    </row>
-    <row r="56" spans="11:16" x14ac:dyDescent="0.2">
-      <c r="K56">
-        <f t="shared" si="0"/>
-        <v>20</v>
+      <c r="K56" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="L56" s="1">
-        <v>1048576</v>
-      </c>
-      <c r="M56" s="1">
-        <v>1024</v>
-      </c>
-      <c r="N56" s="1">
-        <v>64</v>
-      </c>
-      <c r="O56" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P56" s="1">
         <v>0.58847399999999994</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:D1"/>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B10:D10"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>